<commit_message>
Rifatto Eclat sia normale che parallelo
</commit_message>
<xml_diff>
--- a/src/main/resources/results/tempiAlgoritmi.xlsx
+++ b/src/main/resources/results/tempiAlgoritmi.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Universita'\Magistrale - Bologna\2° Anno\I Semestre - 2° Anno\SCP - Scalable And Cloud Computing\Progetto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Universita'\Magistrale - Bologna\2° Anno\I Semestre - 2° Anno\SCP - Scalable And Cloud Computing\Progetto\SCP_DataMiningProject_FP-Growth\src\main\resources\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{398B6E96-C39D-4CF7-8673-A55C9E2B2240}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89E91013-D763-4226-8FCC-62EF8126BB6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{0D229995-9CA3-4D4E-B806-071DE37F7837}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="9072" xr2:uid="{0D229995-9CA3-4D4E-B806-071DE37F7837}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Grandezza Dataset</t>
   </si>
@@ -45,20 +45,23 @@
     <t>Eclat (ms)</t>
   </si>
   <si>
-    <t>x30</t>
-  </si>
-  <si>
     <t>x1</t>
   </si>
   <si>
     <t>Differenza (s)</t>
+  </si>
+  <si>
+    <t>x10</t>
+  </si>
+  <si>
+    <t>Min Support</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -82,21 +85,52 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="17"/>
+      <b/>
+      <sz val="16"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="17"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor theme="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -104,11 +138,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -116,14 +159,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -131,13 +180,49 @@
   </cellStyles>
   <dxfs count="6">
     <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -153,13 +238,23 @@
         <vertAlign val="baseline"/>
         <sz val="17"/>
         <color auto="1"/>
-        <name val="Calibri"/>
+        <name val="Arial"/>
         <family val="2"/>
-        <scheme val="minor"/>
+        <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
       <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -194,14 +289,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C9D35DCE-1631-436D-95C3-139F381DCC05}" name="Tabella3" displayName="Tabella3" ref="B2:E4" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="B2:E4" xr:uid="{C9D35DCE-1631-436D-95C3-139F381DCC05}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C9D35DCE-1631-436D-95C3-139F381DCC05}" name="Tabella3" displayName="Tabella3" ref="C2:F4" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="C2:F4" xr:uid="{C9D35DCE-1631-436D-95C3-139F381DCC05}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{4524534B-3CFA-409B-ADEE-DEB9ACDDB4E0}" name="Grandezza Dataset" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{3CD426B1-529D-4A1B-B8E4-1F062DDF1858}" name="Eclat (ms)" dataDxfId="2"/>
     <tableColumn id="3" xr3:uid="{DBFFC6E7-506D-4F08-BEDD-67A922C140AD}" name="Eclat Parallelo (ms)" dataDxfId="1"/>
     <tableColumn id="4" xr3:uid="{2B97BA95-4C34-4825-9C96-3DCBA2C14C89}" name="Differenza (s)" dataDxfId="0">
-      <calculatedColumnFormula>(C3-D3)/1000</calculatedColumnFormula>
+      <calculatedColumnFormula>(D3-E3)/1000</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -505,66 +600,77 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB5AD1EA-6335-44D6-9470-F3383820DCD1}">
-  <dimension ref="B2:E11"/>
+  <dimension ref="B2:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="34" customWidth="1"/>
-    <col min="3" max="5" width="25.77734375" customWidth="1"/>
+    <col min="2" max="2" width="23.21875" customWidth="1"/>
+    <col min="3" max="3" width="34" customWidth="1"/>
+    <col min="4" max="6" width="25.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="2:6" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="7">
+        <v>3</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="6">
+        <v>4251</v>
+      </c>
+      <c r="E3" s="6">
+        <v>4159</v>
+      </c>
+      <c r="F3" s="6">
+        <f t="shared" ref="F3:F4" si="0">(D3-E3)/1000</f>
+        <v>9.1999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="7"/>
+      <c r="C4" s="5" t="s">
         <v>5</v>
       </c>
+      <c r="D4" s="6">
+        <v>50631</v>
+      </c>
+      <c r="E4" s="6">
+        <v>38178</v>
+      </c>
+      <c r="F4" s="6">
+        <f t="shared" si="0"/>
+        <v>12.452999999999999</v>
+      </c>
     </row>
-    <row r="3" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="5">
-        <v>33126</v>
-      </c>
-      <c r="D3" s="5">
-        <v>5736</v>
-      </c>
-      <c r="E3" s="5">
-        <f t="shared" ref="E3:E4" si="0">(C3-D3)/1000</f>
-        <v>27.39</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="5">
-        <v>319500</v>
-      </c>
-      <c r="D4" s="5">
-        <v>53198</v>
-      </c>
-      <c r="E4" s="5">
-        <f t="shared" si="0"/>
-        <v>266.30200000000002</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C11" s="4"/>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D11" s="3"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B3:B4"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Migliorato di gran lunga entrambi gli algoritmi Eclat. Ora non vengono più usati i for
</commit_message>
<xml_diff>
--- a/src/main/resources/results/tempiAlgoritmi.xlsx
+++ b/src/main/resources/results/tempiAlgoritmi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Universita'\Magistrale - Bologna\2° Anno\I Semestre - 2° Anno\SCP - Scalable And Cloud Computing\Progetto\SCP_DataMiningProject_FP-Growth\src\main\resources\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89E91013-D763-4226-8FCC-62EF8126BB6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47CFA83D-8695-4658-B944-1E7859639D0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="9072" xr2:uid="{0D229995-9CA3-4D4E-B806-071DE37F7837}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{0D229995-9CA3-4D4E-B806-071DE37F7837}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -603,7 +603,7 @@
   <dimension ref="B2:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -632,20 +632,20 @@
     </row>
     <row r="3" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="7">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="6">
-        <v>4251</v>
+        <v>1145</v>
       </c>
       <c r="E3" s="6">
-        <v>4159</v>
+        <v>921</v>
       </c>
       <c r="F3" s="6">
         <f t="shared" ref="F3:F4" si="0">(D3-E3)/1000</f>
-        <v>9.1999999999999998E-2</v>
+        <v>0.224</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -654,14 +654,14 @@
         <v>5</v>
       </c>
       <c r="D4" s="6">
-        <v>50631</v>
+        <v>7528</v>
       </c>
       <c r="E4" s="6">
-        <v>38178</v>
+        <v>3274</v>
       </c>
       <c r="F4" s="6">
         <f t="shared" si="0"/>
-        <v>12.452999999999999</v>
+        <v>4.2539999999999996</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.3">

</xml_diff>